<commit_message>
concept closure, runs again.
</commit_message>
<xml_diff>
--- a/model_sets/src/current.xlsx
+++ b/model_sets/src/current.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -50,6 +50,12 @@
     <t xml:space="preserve">current</t>
   </si>
   <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test summary</t>
+  </si>
+  <si>
     <t xml:space="preserve">package</t>
   </si>
   <si>
@@ -57,6 +63,21 @@
   </si>
   <si>
     <t xml:space="preserve">related</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specimen description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default:C:Thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default:C:Thing, default:c:Thing</t>
   </si>
   <si>
     <t xml:space="preserve">parent</t>
@@ -180,7 +201,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -230,10 +251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -256,6 +277,14 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -274,17 +303,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -296,10 +325,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -309,6 +338,26 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -337,7 +386,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -349,19 +398,19 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -399,16 +448,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -417,13 +466,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Travis build of master
</commit_message>
<xml_diff>
--- a/model_sets/src/current.xlsx
+++ b/model_sets/src/current.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="model" r:id="rId8" sheetId="6"/>
-    <sheet name="packages" r:id="rId9" sheetId="7"/>
-    <sheet name="concepts" r:id="rId10" sheetId="8"/>
-    <sheet name="elements" r:id="rId11" sheetId="9"/>
-    <sheet name="structures" r:id="rId12" sheetId="10"/>
+    <sheet name="model" r:id="rId8" sheetId="11"/>
+    <sheet name="packages" r:id="rId9" sheetId="12"/>
+    <sheet name="concepts" r:id="rId10" sheetId="13"/>
+    <sheet name="elements" r:id="rId11" sheetId="14"/>
+    <sheet name="structures" r:id="rId12" sheetId="15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="40">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -218,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,6 +226,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment wrapText="true"/>
@@ -242,79 +245,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" style="2" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="2" width="8.21875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="2" width="7.8203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="2" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="2" width="8.4609375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="2" width="14.140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="2" width="15.09765625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="2" width="5.046875" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -325,14 +256,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="7.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="2" width="21.484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="2" width="22.88671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="2" width="11.0078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="2" width="7.02734375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="2" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="3" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="21.484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="3" width="22.88671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="3" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="3" width="11.0078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="3" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="3" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="3" width="0.94921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -357,9 +288,6 @@
       <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -392,9 +320,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -403,13 +331,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="2" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="2" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="3" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="3" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="3" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="3" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="3" width="5.5703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -431,18 +358,15 @@
       <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -451,16 +375,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="2" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="2" width="7.31640625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="2" width="6.87890625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="2" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="3" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="3" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="3" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="3" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="3" width="7.31640625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="3" width="6.87890625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="3" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="3" width="5.5703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -491,18 +414,15 @@
       <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -511,19 +431,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="2" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="2" width="6.44921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="2" width="8.4609375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="2" width="15.5390625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="2" width="14.140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="2" width="6.87890625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="2" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="3" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="3" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="3" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="3" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="3" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="3" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="3" width="15.5390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="3" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="3" width="6.87890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="3" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="3" width="5.5703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -563,8 +482,73 @@
       <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
-        <v>25</v>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" style="3" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="3" width="8.21875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="3" width="7.8203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="3" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="3" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="3" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="3" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="3" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="3" width="15.09765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="3" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="3" width="5.5703125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setting up travis full workflow
</commit_message>
<xml_diff>
--- a/model_sets/src/current.xlsx
+++ b/model_sets/src/current.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="model" r:id="rId8" sheetId="26"/>
-    <sheet name="packages" r:id="rId9" sheetId="27"/>
-    <sheet name="concepts" r:id="rId10" sheetId="28"/>
-    <sheet name="elements" r:id="rId11" sheetId="29"/>
-    <sheet name="structures" r:id="rId12" sheetId="30"/>
+    <sheet name="model" r:id="rId8" sheetId="6"/>
+    <sheet name="packages" r:id="rId9" sheetId="7"/>
+    <sheet name="concepts" r:id="rId10" sheetId="8"/>
+    <sheet name="elements" r:id="rId11" sheetId="9"/>
+    <sheet name="structures" r:id="rId12" sheetId="10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="40">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -218,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,18 +226,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment wrapText="true"/>
@@ -254,9 +242,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -265,49 +253,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="6" width="7.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="6" width="21.484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="6" width="22.88671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="11.0078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="6" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="2" width="8.21875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="2" width="7.8203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="2" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="2" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="2" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="2" width="15.09765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="2" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -315,9 +314,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -326,9 +325,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="6" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="2" width="21.484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="2" width="22.88671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="2" width="11.0078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="2" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="2" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -341,15 +345,56 @@
       <c r="C1" t="s">
         <v>20</v>
       </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -358,32 +403,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="6" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="6" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="6" width="7.31640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="2" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="2" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -391,9 +440,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -402,15 +451,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="6" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="6" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="6" width="6.44921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="6" width="8.4609375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="6" width="15.5390625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="6" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="2" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="2" width="7.31640625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="2" width="6.87890625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="2" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -430,16 +480,19 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -447,9 +500,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -458,15 +511,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="6" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="6" width="8.21875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="6" width="7.8203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="6" width="8.4609375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="6" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="2" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="2" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="2" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="2" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="2" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="2" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="2" width="15.5390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="2" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="2" width="6.87890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="2" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="2" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="2" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -477,25 +534,37 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
         <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring, before trying to run.
</commit_message>
<xml_diff>
--- a/model_sets/src/current.xlsx
+++ b/model_sets/src/current.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="model" r:id="rId8" sheetId="31"/>
-    <sheet name="packages" r:id="rId9" sheetId="32"/>
-    <sheet name="concepts" r:id="rId10" sheetId="33"/>
-    <sheet name="elements" r:id="rId11" sheetId="34"/>
-    <sheet name="structures" r:id="rId12" sheetId="35"/>
+    <sheet name="model" r:id="rId8" sheetId="26"/>
+    <sheet name="packages" r:id="rId9" sheetId="27"/>
+    <sheet name="concepts" r:id="rId10" sheetId="28"/>
+    <sheet name="elements" r:id="rId11" sheetId="29"/>
+    <sheet name="structures" r:id="rId12" sheetId="30"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="40">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -218,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,9 +226,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment wrapText="true"/>
@@ -257,7 +254,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -268,14 +265,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="7" width="7.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="7" width="21.484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="7" width="22.88671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="7" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="7" width="11.0078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="7.02734375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="7" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="7" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="6" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="6" width="21.484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="6" width="22.88671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="11.0078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="6" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="6" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="6" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -335,7 +332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -346,13 +343,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="7" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="7" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="7" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="7" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="7" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="7" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="6" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="6" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="6" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -383,7 +380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -394,16 +391,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="7" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="7" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="7" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="7" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="7" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="7.31640625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="7" width="6.87890625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="7" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="7" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="7" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="6" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="6" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="6" width="7.31640625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="6" width="6.87890625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="6" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="6" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="6" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -443,7 +440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -454,19 +451,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="7" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="7" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="7" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="7" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="7" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="6.44921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="7" width="8.4609375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="7" width="15.5390625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="7" width="14.140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="7" width="6.87890625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="7" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="7" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="7" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="6" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="6" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="6" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="6" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="6" width="15.5390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="6" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="6" width="6.87890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="6" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="6" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="6" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -515,7 +512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -526,19 +523,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="7" width="8.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="7" width="5.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="7" width="8.21875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="7" width="7.8203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="7" width="8.8125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="10.21484375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="7" width="8.17578125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="7" width="8.4609375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="7" width="14.140625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="7" width="15.09765625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="7" width="6.0703125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="7" width="5.5703125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="7" width="5.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="6" width="8.015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="6" width="5.67578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="6" width="8.21875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="6" width="7.8203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="6" width="10.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="6" width="8.17578125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="6" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="6" width="14.140625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="6" width="15.09765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="6" width="6.0703125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="6" width="5.5703125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="6" width="5.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>